<commit_message>
Excel basics done - along with Exercise 101.
</commit_message>
<xml_diff>
--- a/Excel_101.xlsx
+++ b/Excel_101.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Desktop\Data Science\ZTM_Excel_Mastery\Notebook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Desktop\Data Science\ZTM_Excel_Mastery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53E0663-A936-4B16-A333-A22D8F527541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B1127A-A4DC-4594-A052-6C5E85065FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1044" yWindow="348" windowWidth="11040" windowHeight="8184" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Passion-Fruit</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>02/12/2021</t>
+  </si>
+  <si>
+    <t>MERGED</t>
   </si>
 </sst>
 </file>
@@ -93,7 +96,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="167" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -118,7 +121,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -126,16 +129,100 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,6 +514,7 @@
     <col min="1" max="1" width="15.44140625" customWidth="1"/>
     <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="7" max="7" width="12.5546875" customWidth="1"/>
   </cols>
@@ -586,7 +674,7 @@
         <v>44206</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -595,16 +683,43 @@
       </c>
       <c r="C13" s="1">
         <v>44197</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1111</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D15" s="11"/>
+      <c r="E15" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>1111.7660000000001</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="9">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
@@ -612,7 +727,21 @@
         <v>19</v>
       </c>
     </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>44228</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="D14:D16"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>